<commit_message>
Updated the validation for combined and showcase scenarios.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/CombinedValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/CombinedValidation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Source\engine\test\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCB2B50-9EFC-4FBF-B9D5-4C71E817894C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DB0034-6766-43E5-B8BC-FC0084E286B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13785" yWindow="5670" windowWidth="32670" windowHeight="23535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -33,7 +33,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -874,7 +876,7 @@
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1022,6 +1024,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1408,7 +1413,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,13 +1519,13 @@
         <v>78</v>
       </c>
       <c r="F3" s="41">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G3" s="40" t="s">
         <v>85</v>
       </c>
       <c r="H3" s="42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3" s="40" t="s">
         <v>86</v>
@@ -1688,14 +1693,14 @@
       </c>
       <c r="F8" s="47">
         <f>SUM(F3:F7)</f>
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G8" s="44" t="s">
         <v>85</v>
       </c>
       <c r="H8" s="48">
         <f>SUM(H3:H7)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I8" s="44" t="s">
         <v>86</v>
@@ -1725,8 +1730,8 @@
   </sheetPr>
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2138,7 @@
       <c r="I7" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="J7" s="50" t="s">
         <v>76</v>
       </c>
       <c r="K7" s="24" t="s">
@@ -2145,7 +2150,7 @@
       <c r="M7" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="N7" s="50" t="s">
         <v>76</v>
       </c>
       <c r="O7" s="24" t="s">
@@ -2319,7 +2324,7 @@
   </sheetPr>
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -2712,7 +2717,7 @@
   </sheetPr>
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -3168,7 +3173,7 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -3683,7 +3688,7 @@
   </sheetPr>
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the combined scenarios to use supplemental oxygen and mechanical ventilator instead of anesthesia machine. Except the Nathan scenarios which uses the anesthesa machine with an equipment failure.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/CombinedValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/CombinedValidation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DB0034-6766-43E5-B8BC-FC0084E286B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011BF46B-0ADD-4C6D-90BF-8EACE330BB40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6330" yWindow="2340" windowWidth="24825" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="106">
   <si>
     <t>Notes</t>
   </si>
@@ -153,12 +153,6 @@
     <t>Represents suctioning</t>
   </si>
   <si>
-    <t>Ventilate w/ O2 tank</t>
-  </si>
-  <si>
-    <t>O2 Source is set to Tank 1</t>
-  </si>
-  <si>
     <t>Intubate</t>
   </si>
   <si>
@@ -324,9 +318,6 @@
     <t xml:space="preserve">Continues to decrease because still fully blocked  </t>
   </si>
   <si>
-    <t xml:space="preserve">Ventilator On; therefore, 16  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Begins to increase because airway obstruction is cleared  </t>
   </si>
   <si>
@@ -351,12 +342,6 @@
     <t>Slight decrease to due anesthesia machine resistance    NC @cite dukeSME</t>
   </si>
   <si>
-    <t>Administer Etomidate - 27 mg</t>
-  </si>
-  <si>
-    <t>No Etomidate in drug directory, so we use Ketamine instead; Drug Onset &lt; 1 minute</t>
-  </si>
-  <si>
     <t>Administer Succinylcholine - 115 mg</t>
   </si>
   <si>
@@ -364,6 +349,18 @@
   </si>
   <si>
     <t>Administer Succinylcholine - 100mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventilator On; therefore, 14  </t>
+  </si>
+  <si>
+    <t>Ventilate w/ Mask</t>
+  </si>
+  <si>
+    <t>Administer Ketamine - 27 mg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Drug Onset &lt; 1 minute</t>
   </si>
 </sst>
 </file>
@@ -1412,7 +1409,7 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1434,283 +1431,283 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>21</v>
       </c>
       <c r="C1" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>22</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="39" t="s">
-        <v>84</v>
-      </c>
       <c r="K1" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" s="38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" s="38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I2" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J2" s="38" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K2" s="35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="20" t="s">
         <v>24</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F3" s="41">
         <v>28</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H3" s="42">
         <v>2</v>
       </c>
       <c r="I3" s="40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J3" s="43">
         <v>0</v>
       </c>
       <c r="K3" s="40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="20" t="s">
         <v>25</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F4" s="41">
         <v>25</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H4" s="42">
         <v>0</v>
       </c>
       <c r="I4" s="40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J4" s="43">
         <v>0</v>
       </c>
       <c r="K4" s="40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="41">
         <v>20</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H5" s="42">
         <v>0</v>
       </c>
       <c r="I5" s="40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J5" s="43">
         <v>0</v>
       </c>
       <c r="K5" s="40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>29</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="20" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F6" s="41">
         <v>20</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H6" s="42">
         <v>0</v>
       </c>
       <c r="I6" s="40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J6" s="43">
         <v>0</v>
       </c>
       <c r="K6" s="40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="20" t="s">
         <v>32</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F7" s="41">
         <v>30</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H7" s="42">
         <v>0</v>
       </c>
       <c r="I7" s="40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J7" s="43">
         <v>0</v>
       </c>
       <c r="K7" s="40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="46"/>
       <c r="C8" s="44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E8" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F8" s="47">
         <f>SUM(F3:F7)</f>
         <v>123</v>
       </c>
       <c r="G8" s="44" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H8" s="48">
         <f>SUM(H3:H7)</f>
         <v>2</v>
       </c>
       <c r="I8" s="44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J8" s="49">
         <f>SUM(J3:J7)</f>
         <v>0</v>
       </c>
       <c r="K8" s="44" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1730,8 +1727,8 @@
   </sheetPr>
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1760,470 +1757,470 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="12" t="s">
+      <c r="M1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="16" t="s">
+      <c r="O1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="16" t="s">
+      <c r="Q1" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="27" t="s">
-        <v>46</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>45</v>
-      </c>
       <c r="S1" s="27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>28</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3" s="19">
         <v>30</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H3" s="19">
         <v>90</v>
       </c>
       <c r="I3" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="S3" s="26" t="s">
         <v>78</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="K3" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="O3" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q3" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="S3" s="26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F4" s="9">
         <v>90</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" s="9">
         <v>240</v>
       </c>
       <c r="I4" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="S4" s="26" t="s">
         <v>78</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="K4" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q4" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="S4" s="26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" s="9">
         <v>240</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H5" s="9">
         <v>250</v>
       </c>
       <c r="I5" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q5" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="S5" s="26" t="s">
         <v>78</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K5" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="M5" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q5" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="S5" s="26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" s="9">
         <v>250</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H6" s="9">
         <v>310</v>
       </c>
       <c r="I6" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M6" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O6" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="S6" s="26" t="s">
         <v>78</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="K6" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="M6" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="O6" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="P6" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q6" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="S6" s="26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F7" s="9">
         <v>310</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" s="9">
         <v>400</v>
       </c>
       <c r="I7" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q7" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="S7" s="26" t="s">
         <v>78</v>
-      </c>
-      <c r="J7" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="K7" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="M7" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="N7" s="50" t="s">
-        <v>76</v>
-      </c>
-      <c r="O7" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q7" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="R7" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="S7" s="26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F8" s="9">
         <v>400</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H8" s="9">
         <v>900</v>
       </c>
       <c r="I8" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q8" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="S8" s="26" t="s">
         <v>78</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="M8" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="O8" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="P8" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="Q8" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="R8" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="S8" s="26" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -2324,8 +2321,8 @@
   </sheetPr>
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2354,350 +2351,350 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="12" t="s">
+      <c r="M1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="31" t="s">
+      <c r="O1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="31" t="s">
+      <c r="Q1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>45</v>
-      </c>
       <c r="S1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3" s="2">
         <v>30</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H3" s="2">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O3" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P3" s="32" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="Q3" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R3" s="8">
         <v>100</v>
       </c>
       <c r="S3" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="34" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F4" s="2">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" s="2">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="I4" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="O4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S4" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="M4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="O4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="S4" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="34"/>
       <c r="E5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" s="2">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H5" s="2">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="I5" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="S5" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="S5" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="34"/>
       <c r="E6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" s="2">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H6" s="2">
-        <v>770</v>
+        <v>725</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O6" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P6" s="11">
         <v>16</v>
       </c>
       <c r="Q6" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="S6" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2717,8 +2714,8 @@
   </sheetPr>
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2747,413 +2744,413 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="12" t="s">
+      <c r="M1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="31" t="s">
+      <c r="O1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="31" t="s">
+      <c r="Q1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>45</v>
-      </c>
       <c r="S1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="34"/>
       <c r="E3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3" s="2">
         <v>30</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H3" s="2">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="I3" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="O3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="S3" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="34" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F4" s="2">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" s="2">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="I4" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="S4" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="M4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="O4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="S4" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" s="2">
+        <v>100</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="2">
         <v>130</v>
       </c>
-      <c r="G5" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="2">
-        <v>160</v>
-      </c>
       <c r="I5" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="S5" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="O5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P5" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="S5" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" s="2">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H6" s="2">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K6" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M6" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N6" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="O6" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P6" s="11">
         <v>16</v>
       </c>
       <c r="Q6" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="S6" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>16</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F7" s="2">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" s="2">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="I7" s="29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K7" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M7" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N7" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="O7" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="P7" s="11">
         <v>16</v>
       </c>
       <c r="Q7" s="29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="S7" s="29" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -3173,8 +3170,8 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3203,472 +3200,470 @@
   <sheetData>
     <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="12" t="s">
+      <c r="M1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="31" t="s">
+      <c r="O1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="31" t="s">
+      <c r="Q1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>45</v>
-      </c>
       <c r="S1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3" s="34">
         <v>30</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H3" s="34">
         <v>150</v>
       </c>
       <c r="I3" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="M3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="O3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="S3" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>34</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="34" t="s">
         <v>35</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F4" s="34">
         <v>150</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" s="34">
         <v>210</v>
       </c>
       <c r="I4" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="S4" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="M4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R4" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="S4" s="29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>36</v>
+        <v>103</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>37</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="D5" s="34"/>
       <c r="E5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" s="34">
         <v>210</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H5" s="34">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="I5" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S5" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="J5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="O5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="S5" s="29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" s="34">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H6" s="34">
-        <v>290</v>
+        <v>245</v>
       </c>
       <c r="I6" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q6" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="S6" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="K6" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="M6" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="O6" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P6" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q6" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="S6" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F7" s="34">
-        <v>290</v>
+        <v>245</v>
       </c>
       <c r="G7" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H7" s="34">
-        <v>320</v>
+        <v>275</v>
       </c>
       <c r="I7" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K7" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O7" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q7" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="S7" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="K7" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L7" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="M7" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="O7" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q7" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R7" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="S7" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F8" s="34">
-        <v>320</v>
+        <v>275</v>
       </c>
       <c r="G8" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H8" s="34">
-        <v>520</v>
+        <v>475</v>
       </c>
       <c r="I8" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="O8" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q8" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="S8" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="M8" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="O8" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P8" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q8" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R8" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="S8" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3718,350 +3713,350 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D1" s="30" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" s="12" t="s">
+      <c r="M1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="31" t="s">
+      <c r="O1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="M1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="31" t="s">
+      <c r="Q1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="P1" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="R1" s="31" t="s">
-        <v>45</v>
-      </c>
       <c r="S1" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="O2" s="29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="S2" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="34" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" s="34" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3" s="2">
         <v>30</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H3" s="2">
         <v>120</v>
       </c>
       <c r="I3" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q3" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="S3" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="K3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="M3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="O3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P3" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q3" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="S3" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F4" s="2">
         <v>120</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" s="2">
         <v>210</v>
       </c>
       <c r="I4" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="S4" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="O4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q4" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="S4" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" s="2">
         <v>210</v>
       </c>
       <c r="G5" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H5" s="2">
         <v>340</v>
       </c>
       <c r="I5" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="S5" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="O5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q5" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R5" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="S5" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="34" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" s="2">
         <v>340</v>
       </c>
       <c r="G6" s="33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H6" s="2">
         <v>840</v>
       </c>
       <c r="I6" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q6" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="R6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="S6" s="29" t="s">
         <v>78</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="K6" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="O6" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="P6" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="S6" s="29" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated combat multitrauma scenario and system methodology. Final clean up of the heat stroke and combined scenarios. Added references to Source.bib.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/CombinedValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/CombinedValidation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011BF46B-0ADD-4C6D-90BF-8EACE330BB40}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B540A0-83C6-4BEC-A7CE-D2C6A6B10FE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="2340" windowWidth="24825" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3195" yWindow="6285" windowWidth="24825" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -1727,8 +1727,8 @@
   </sheetPr>
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:S8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2321,7 +2321,7 @@
   </sheetPr>
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:S6"/>
     </sheetView>
   </sheetViews>
@@ -3170,8 +3170,8 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:S8"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Documentation edits. Minor typos, etc.
</commit_message>
<xml_diff>
--- a/data/human/adult/validation/Scenarios/CombinedValidation.xlsx
+++ b/data/human/adult/validation/Scenarios/CombinedValidation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PulsePhysiologyEngine\data\human\adult\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B540A0-83C6-4BEC-A7CE-D2C6A6B10FE2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819FFA86-242D-4D39-A0F0-433A9E074658}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="6285" windowWidth="24825" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="24825" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -1409,8 +1409,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,13 +1516,13 @@
         <v>76</v>
       </c>
       <c r="F3" s="41">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G3" s="40" t="s">
         <v>83</v>
       </c>
       <c r="H3" s="42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I3" s="40" t="s">
         <v>84</v>
@@ -1690,14 +1690,14 @@
       </c>
       <c r="F8" s="47">
         <f>SUM(F3:F7)</f>
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G8" s="44" t="s">
         <v>83</v>
       </c>
       <c r="H8" s="48">
         <f>SUM(H3:H7)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I8" s="44" t="s">
         <v>84</v>
@@ -1727,7 +1727,7 @@
   </sheetPr>
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>

</xml_diff>